<commit_message>
Added Collable Test cases and Have done code optimization
</commit_message>
<xml_diff>
--- a/BSFPilotEngagement/templates/test1.xlsx
+++ b/BSFPilotEngagement/templates/test1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chilu\git\repository\BSFPilotEngagement\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35FAB7F-3AC2-43B3-9A8D-62F13C50CC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7FEC81-2EE7-422D-8DC3-4E289E7AC1D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="8" xr2:uid="{D9395F2A-E6BF-48EE-9790-87FB8BBF8441}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{D9395F2A-E6BF-48EE-9790-87FB8BBF8441}"/>
   </bookViews>
   <sheets>
     <sheet name="1061" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="2203" sheetId="10" r:id="rId7"/>
     <sheet name="2873" sheetId="8" r:id="rId8"/>
     <sheet name="1800" sheetId="9" r:id="rId9"/>
-    <sheet name="Sheet1" sheetId="11" r:id="rId10"/>
+    <sheet name="21082" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="70">
   <si>
     <t>AcceptsAutomation</t>
   </si>
@@ -133,12 +133,6 @@
     <t>OH</t>
   </si>
   <si>
-    <t>TSG</t>
-  </si>
-  <si>
-    <t>STG1</t>
-  </si>
-  <si>
     <t>Samsung</t>
   </si>
   <si>
@@ -187,12 +181,6 @@
     <t>A. Brooke Phelps</t>
   </si>
   <si>
-    <t>Brain</t>
-  </si>
-  <si>
-    <t>hell123</t>
-  </si>
-  <si>
     <t>Flipkart</t>
   </si>
   <si>
@@ -214,9 +202,6 @@
     <t>Micha Alt</t>
   </si>
   <si>
-    <t>Hekk</t>
-  </si>
-  <si>
     <t>Tiktok</t>
   </si>
   <si>
@@ -256,7 +241,22 @@
     <t>Cynthia Stallworth 507946</t>
   </si>
   <si>
-    <t>Atlass</t>
+    <t>Lotus</t>
+  </si>
+  <si>
+    <t>Tesla</t>
+  </si>
+  <si>
+    <t>Tat</t>
+  </si>
+  <si>
+    <t>Kignfisher</t>
+  </si>
+  <si>
+    <t>Airline</t>
+  </si>
+  <si>
+    <t>Jet_5345</t>
   </si>
 </sst>
 </file>
@@ -613,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09885966-16F7-43D5-8F8D-B8BE03ED6209}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,16 +684,16 @@
         <v>16</v>
       </c>
       <c r="R1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="S1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U1" t="s">
         <v>33</v>
-      </c>
-      <c r="T1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="45" x14ac:dyDescent="0.25">
@@ -704,19 +704,19 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="H2">
         <v>3241</v>
@@ -749,7 +749,7 @@
         <v>27</v>
       </c>
       <c r="R2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="S2">
         <v>1</v>
@@ -768,12 +768,151 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31CE174A-730B-46FF-BD3E-2A5CDEA9B175}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U1" t="s">
+        <v>33</v>
+      </c>
+      <c r="V1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2">
+        <v>3232</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2">
+        <v>44094</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>55</v>
+      </c>
+      <c r="R2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -782,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D48D8D3-FB28-4348-AB39-26B4C38F66CB}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:R2"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,7 +935,8 @@
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="10" max="10" width="21.7109375" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="19" max="19" width="13.140625" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" customWidth="1"/>
+    <col min="22" max="22" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -849,30 +989,30 @@
         <v>3</v>
       </c>
       <c r="Q1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U1" t="s">
+        <v>33</v>
+      </c>
+      <c r="V1" t="s">
         <v>4</v>
-      </c>
-      <c r="R1" t="s">
-        <v>59</v>
-      </c>
-      <c r="S1" t="s">
-        <v>32</v>
-      </c>
-      <c r="T1" t="s">
-        <v>33</v>
-      </c>
-      <c r="U1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2">
         <v>3232</v>
@@ -917,22 +1057,22 @@
         <v>20</v>
       </c>
       <c r="Q2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="R2" t="s">
-        <v>60</v>
-      </c>
-      <c r="S2" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
       </c>
       <c r="T2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U2">
-        <v>2</v>
-      </c>
-      <c r="V2">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="V2" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -944,8 +1084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E5A4907-8EB7-41C8-A757-0F3C4222D6A7}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1:V2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,30 +1146,30 @@
         <v>4</v>
       </c>
       <c r="R1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" t="s">
         <v>32</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>33</v>
       </c>
-      <c r="T1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U1" t="s">
-        <v>35</v>
-      </c>
       <c r="V1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
         <v>36</v>
-      </c>
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" t="s">
-        <v>38</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -1071,22 +1211,22 @@
         <v>20</v>
       </c>
       <c r="Q2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="R2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="S2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1098,8 +1238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB0543E-C0C8-4186-93D3-1700F611353F}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,30 +1297,30 @@
         <v>4</v>
       </c>
       <c r="R1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" t="s">
         <v>32</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>33</v>
       </c>
-      <c r="T1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U1" t="s">
-        <v>35</v>
-      </c>
       <c r="V1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
         <v>39</v>
-      </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -1222,22 +1362,22 @@
         <v>20</v>
       </c>
       <c r="Q2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="R2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="S2">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="T2">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="U2">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="V2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1249,11 +1389,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1116489-9EC7-4ACC-87AF-D085A86A1966}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1:V2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="22" max="22" width="36.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1308,30 +1451,30 @@
         <v>4</v>
       </c>
       <c r="R1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" t="s">
         <v>32</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>33</v>
       </c>
-      <c r="T1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U1" t="s">
-        <v>35</v>
-      </c>
       <c r="V1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
         <v>42</v>
-      </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" t="s">
-        <v>44</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -1373,10 +1516,10 @@
         <v>20</v>
       </c>
       <c r="Q2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="R2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="S2">
         <v>25</v>
@@ -1388,7 +1531,7 @@
         <v>10</v>
       </c>
       <c r="V2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1401,8 +1544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FDEF43-60C4-4153-B470-5B2596E99642}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1449,18 +1592,18 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -1490,7 +1633,7 @@
         <v>27</v>
       </c>
       <c r="M2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1548,13 +1691,13 @@
     </row>
     <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -1593,7 +1736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A94F4A-E054-4F0F-AECA-17BFFA43F9E6}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V1" sqref="V1:V2"/>
     </sheetView>
   </sheetViews>
@@ -1652,30 +1795,30 @@
         <v>4</v>
       </c>
       <c r="R1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" t="s">
         <v>32</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>33</v>
       </c>
-      <c r="T1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U1" t="s">
-        <v>35</v>
-      </c>
       <c r="V1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -1717,10 +1860,10 @@
         <v>20</v>
       </c>
       <c r="Q2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="R2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="S2">
         <v>5</v>
@@ -1732,7 +1875,7 @@
         <v>2</v>
       </c>
       <c r="V2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1744,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E37DA58E-BC19-4E69-BBA2-F37932DF7060}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1809,39 +1952,39 @@
         <v>4</v>
       </c>
       <c r="R1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" t="s">
         <v>32</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>33</v>
       </c>
-      <c r="T1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U1" t="s">
-        <v>35</v>
-      </c>
       <c r="V1" t="s">
+        <v>54</v>
+      </c>
+      <c r="W1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X1" t="s">
         <v>59</v>
       </c>
-      <c r="W1" t="s">
-        <v>63</v>
-      </c>
-      <c r="X1" t="s">
-        <v>64</v>
-      </c>
       <c r="Y1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -1883,10 +2026,10 @@
         <v>20</v>
       </c>
       <c r="Q2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="R2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="S2">
         <v>1</v>
@@ -1898,16 +2041,16 @@
         <v>1</v>
       </c>
       <c r="V2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="W2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="X2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="Y2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>